<commit_message>
Fetch database from Google Sheets
</commit_message>
<xml_diff>
--- a/scripts/officials.xlsx
+++ b/scripts/officials.xlsx
@@ -11411,7 +11411,7 @@
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="2" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="2" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -11441,7 +11441,7 @@
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="2" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="2" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -11456,7 +11456,7 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="2" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="2" fillId="9" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -22928,7 +22928,7 @@
       <c r="D279" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="E279" s="15" t="s">
+      <c r="E279" s="20" t="s">
         <v>483</v>
       </c>
       <c r="F279" s="16" t="s">
@@ -24382,7 +24382,7 @@
       <c r="D315" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E315" s="15" t="s">
+      <c r="E315" s="20" t="s">
         <v>550</v>
       </c>
       <c r="F315" s="16" t="s">
@@ -24426,7 +24426,7 @@
       <c r="D316" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E316" s="15" t="s">
+      <c r="E316" s="20" t="s">
         <v>553</v>
       </c>
       <c r="F316" s="16" t="s">
@@ -24470,7 +24470,7 @@
       <c r="D317" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E317" s="15" t="s">
+      <c r="E317" s="20" t="s">
         <v>556</v>
       </c>
       <c r="F317" s="16" t="s">
@@ -24514,7 +24514,7 @@
       <c r="D318" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E318" s="15" t="s">
+      <c r="E318" s="20" t="s">
         <v>559</v>
       </c>
       <c r="F318" s="16" t="s">
@@ -24558,7 +24558,7 @@
       <c r="D319" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E319" s="15" t="s">
+      <c r="E319" s="20" t="s">
         <v>562</v>
       </c>
       <c r="F319" s="16" t="s">
@@ -24602,7 +24602,7 @@
       <c r="D320" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E320" s="15" t="s">
+      <c r="E320" s="20" t="s">
         <v>565</v>
       </c>
       <c r="F320" s="16" t="s">
@@ -24646,7 +24646,7 @@
       <c r="D321" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E321" s="15" t="s">
+      <c r="E321" s="20" t="s">
         <v>568</v>
       </c>
       <c r="F321" s="16" t="s">
@@ -24690,7 +24690,7 @@
       <c r="D322" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E322" s="15" t="s">
+      <c r="E322" s="20" t="s">
         <v>571</v>
       </c>
       <c r="F322" s="16" t="s">
@@ -24778,7 +24778,7 @@
       <c r="D324" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E324" s="15" t="s">
+      <c r="E324" s="20" t="s">
         <v>576</v>
       </c>
       <c r="F324" s="16" t="s">
@@ -24890,7 +24890,7 @@
       <c r="D327" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E327" s="15" t="s">
+      <c r="E327" s="20" t="s">
         <v>580</v>
       </c>
       <c r="F327" s="16" t="s">
@@ -24934,7 +24934,7 @@
       <c r="D328" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E328" s="15" t="s">
+      <c r="E328" s="20" t="s">
         <v>583</v>
       </c>
       <c r="F328" s="16" t="s">
@@ -24978,7 +24978,7 @@
       <c r="D329" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E329" s="15" t="s">
+      <c r="E329" s="20" t="s">
         <v>586</v>
       </c>
       <c r="F329" s="16" t="s">
@@ -25110,7 +25110,7 @@
       <c r="D332" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E332" s="15" t="s">
+      <c r="E332" s="20" t="s">
         <v>592</v>
       </c>
       <c r="F332" s="16" t="s">
@@ -25154,7 +25154,7 @@
       <c r="D333" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E333" s="15" t="s">
+      <c r="E333" s="20" t="s">
         <v>595</v>
       </c>
       <c r="F333" s="16" t="s">
@@ -25198,7 +25198,7 @@
       <c r="D334" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E334" s="15" t="s">
+      <c r="E334" s="20" t="s">
         <v>598</v>
       </c>
       <c r="F334" s="16" t="s">
@@ -25242,7 +25242,7 @@
       <c r="D335" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E335" s="15" t="s">
+      <c r="E335" s="20" t="s">
         <v>601</v>
       </c>
       <c r="F335" s="16" t="s">
@@ -25286,7 +25286,7 @@
       <c r="D336" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E336" s="15" t="s">
+      <c r="E336" s="20" t="s">
         <v>604</v>
       </c>
       <c r="F336" s="16" t="s">
@@ -25330,7 +25330,7 @@
       <c r="D337" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E337" s="15" t="s">
+      <c r="E337" s="20" t="s">
         <v>607</v>
       </c>
       <c r="F337" s="16" t="s">
@@ -25374,7 +25374,7 @@
       <c r="D338" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E338" s="15" t="s">
+      <c r="E338" s="20" t="s">
         <v>610</v>
       </c>
       <c r="F338" s="16" t="s">
@@ -25418,7 +25418,7 @@
       <c r="D339" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E339" s="15" t="s">
+      <c r="E339" s="20" t="s">
         <v>613</v>
       </c>
       <c r="F339" s="16" t="s">
@@ -25496,7 +25496,7 @@
       <c r="D341" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E341" s="15" t="s">
+      <c r="E341" s="20" t="s">
         <v>617</v>
       </c>
       <c r="F341" s="16" t="s">
@@ -25540,7 +25540,7 @@
       <c r="D342" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E342" s="15" t="s">
+      <c r="E342" s="20" t="s">
         <v>620</v>
       </c>
       <c r="F342" s="16" t="s">
@@ -25628,7 +25628,7 @@
       <c r="D344" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E344" s="15" t="s">
+      <c r="E344" s="20" t="s">
         <v>625</v>
       </c>
       <c r="F344" s="16" t="s">
@@ -25886,7 +25886,7 @@
       <c r="D351" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E351" s="15" t="s">
+      <c r="E351" s="20" t="s">
         <v>632</v>
       </c>
       <c r="F351" s="16" t="s">
@@ -25974,7 +25974,7 @@
       <c r="D353" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E353" s="15" t="s">
+      <c r="E353" s="20" t="s">
         <v>636</v>
       </c>
       <c r="F353" s="16" t="s">
@@ -26018,7 +26018,7 @@
       <c r="D354" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E354" s="15" t="s">
+      <c r="E354" s="20" t="s">
         <v>639</v>
       </c>
       <c r="F354" s="16" t="s">
@@ -26062,7 +26062,7 @@
       <c r="D355" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E355" s="15" t="s">
+      <c r="E355" s="20" t="s">
         <v>642</v>
       </c>
       <c r="F355" s="16" t="s">
@@ -26106,7 +26106,7 @@
       <c r="D356" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E356" s="15" t="s">
+      <c r="E356" s="20" t="s">
         <v>645</v>
       </c>
       <c r="F356" s="16" t="s">
@@ -26150,7 +26150,7 @@
       <c r="D357" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E357" s="15" t="s">
+      <c r="E357" s="20" t="s">
         <v>648</v>
       </c>
       <c r="F357" s="16" t="s">
@@ -26194,7 +26194,7 @@
       <c r="D358" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E358" s="15" t="s">
+      <c r="E358" s="20" t="s">
         <v>651</v>
       </c>
       <c r="F358" s="16" t="s">
@@ -26238,7 +26238,7 @@
       <c r="D359" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E359" s="15" t="s">
+      <c r="E359" s="20" t="s">
         <v>654</v>
       </c>
       <c r="F359" s="16" t="s">
@@ -26326,7 +26326,7 @@
       <c r="D361" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E361" s="15" t="s">
+      <c r="E361" s="20" t="s">
         <v>659</v>
       </c>
       <c r="F361" s="16" t="s">
@@ -26370,7 +26370,7 @@
       <c r="D362" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E362" s="15" t="s">
+      <c r="E362" s="20" t="s">
         <v>662</v>
       </c>
       <c r="F362" s="16" t="s">
@@ -26414,7 +26414,7 @@
       <c r="D363" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E363" s="15" t="s">
+      <c r="E363" s="20" t="s">
         <v>665</v>
       </c>
       <c r="F363" s="16" t="s">
@@ -26458,7 +26458,7 @@
       <c r="D364" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E364" s="15" t="s">
+      <c r="E364" s="20" t="s">
         <v>668</v>
       </c>
       <c r="F364" s="16" t="s">
@@ -26502,7 +26502,7 @@
       <c r="D365" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E365" s="15" t="s">
+      <c r="E365" s="20" t="s">
         <v>671</v>
       </c>
       <c r="F365" s="16" t="s">
@@ -26810,7 +26810,7 @@
       <c r="D372" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E372" s="15" t="s">
+      <c r="E372" s="20" t="s">
         <v>684</v>
       </c>
       <c r="F372" s="16" t="s">
@@ -26854,7 +26854,7 @@
       <c r="D373" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E373" s="15" t="s">
+      <c r="E373" s="20" t="s">
         <v>687</v>
       </c>
       <c r="F373" s="16" t="s">
@@ -26942,7 +26942,7 @@
       <c r="D375" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E375" s="15" t="s">
+      <c r="E375" s="20" t="s">
         <v>692</v>
       </c>
       <c r="F375" s="16" t="s">
@@ -26986,7 +26986,7 @@
       <c r="D376" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E376" s="15" t="s">
+      <c r="E376" s="20" t="s">
         <v>695</v>
       </c>
       <c r="F376" s="16" t="s">
@@ -27030,7 +27030,7 @@
       <c r="D377" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E377" s="15" t="s">
+      <c r="E377" s="20" t="s">
         <v>698</v>
       </c>
       <c r="F377" s="16" t="s">
@@ -27074,7 +27074,7 @@
       <c r="D378" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E378" s="15" t="s">
+      <c r="E378" s="20" t="s">
         <v>701</v>
       </c>
       <c r="F378" s="16" t="s">
@@ -27118,7 +27118,7 @@
       <c r="D379" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E379" s="15" t="s">
+      <c r="E379" s="20" t="s">
         <v>704</v>
       </c>
       <c r="F379" s="16" t="s">
@@ -27162,7 +27162,7 @@
       <c r="D380" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E380" s="15" t="s">
+      <c r="E380" s="20" t="s">
         <v>707</v>
       </c>
       <c r="F380" s="16" t="s">
@@ -27206,7 +27206,7 @@
       <c r="D381" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E381" s="15" t="s">
+      <c r="E381" s="20" t="s">
         <v>710</v>
       </c>
       <c r="F381" s="16" t="s">
@@ -27396,7 +27396,7 @@
       <c r="D386" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E386" s="15" t="s">
+      <c r="E386" s="20" t="s">
         <v>718</v>
       </c>
       <c r="F386" s="16" t="s">
@@ -27440,7 +27440,7 @@
       <c r="D387" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E387" s="15" t="s">
+      <c r="E387" s="20" t="s">
         <v>721</v>
       </c>
       <c r="F387" s="16" t="s">
@@ -27484,7 +27484,7 @@
       <c r="D388" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E388" s="15" t="s">
+      <c r="E388" s="20" t="s">
         <v>724</v>
       </c>
       <c r="F388" s="16" t="s">
@@ -27528,7 +27528,7 @@
       <c r="D389" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E389" s="15" t="s">
+      <c r="E389" s="20" t="s">
         <v>727</v>
       </c>
       <c r="F389" s="16" t="s">
@@ -27572,7 +27572,7 @@
       <c r="D390" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E390" s="15" t="s">
+      <c r="E390" s="20" t="s">
         <v>730</v>
       </c>
       <c r="F390" s="16" t="s">
@@ -27616,7 +27616,7 @@
       <c r="D391" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E391" s="15" t="s">
+      <c r="E391" s="20" t="s">
         <v>733</v>
       </c>
       <c r="F391" s="16" t="s">
@@ -27748,7 +27748,7 @@
       <c r="D394" s="14" t="s">
         <v>740</v>
       </c>
-      <c r="E394" s="15" t="s">
+      <c r="E394" s="20" t="s">
         <v>741</v>
       </c>
       <c r="F394" s="16" t="s">
@@ -27792,7 +27792,7 @@
       <c r="D395" s="14" t="s">
         <v>744</v>
       </c>
-      <c r="E395" s="15" t="s">
+      <c r="E395" s="20" t="s">
         <v>745</v>
       </c>
       <c r="F395" s="16" t="s">
@@ -27836,7 +27836,7 @@
       <c r="D396" s="14" t="s">
         <v>748</v>
       </c>
-      <c r="E396" s="15" t="s">
+      <c r="E396" s="20" t="s">
         <v>749</v>
       </c>
       <c r="F396" s="16"/>
@@ -27878,7 +27878,7 @@
       <c r="D397" s="14" t="s">
         <v>751</v>
       </c>
-      <c r="E397" s="15" t="s">
+      <c r="E397" s="20" t="s">
         <v>752</v>
       </c>
       <c r="F397" s="16"/>
@@ -28022,7 +28022,7 @@
       <c r="D401" s="14" t="s">
         <v>756</v>
       </c>
-      <c r="E401" s="15" t="s">
+      <c r="E401" s="20" t="s">
         <v>757</v>
       </c>
       <c r="F401" s="16"/>
@@ -28064,7 +28064,7 @@
       <c r="D402" s="14" t="s">
         <v>759</v>
       </c>
-      <c r="E402" s="15" t="s">
+      <c r="E402" s="20" t="s">
         <v>760</v>
       </c>
       <c r="F402" s="16" t="s">
@@ -28108,7 +28108,7 @@
       <c r="D403" s="14" t="s">
         <v>762</v>
       </c>
-      <c r="E403" s="15" t="s">
+      <c r="E403" s="20" t="s">
         <v>763</v>
       </c>
       <c r="F403" s="16" t="s">
@@ -28186,7 +28186,7 @@
       <c r="D405" s="14" t="s">
         <v>766</v>
       </c>
-      <c r="E405" s="15" t="s">
+      <c r="E405" s="20" t="s">
         <v>767</v>
       </c>
       <c r="F405" s="16" t="s">
@@ -28230,7 +28230,7 @@
       <c r="D406" s="14" t="s">
         <v>770</v>
       </c>
-      <c r="E406" s="15" t="s">
+      <c r="E406" s="20" t="s">
         <v>771</v>
       </c>
       <c r="F406" s="16"/>
@@ -28272,7 +28272,7 @@
       <c r="D407" s="14" t="s">
         <v>773</v>
       </c>
-      <c r="E407" s="15" t="s">
+      <c r="E407" s="20" t="s">
         <v>774</v>
       </c>
       <c r="F407" s="16" t="s">
@@ -28316,7 +28316,7 @@
       <c r="D408" s="14" t="s">
         <v>776</v>
       </c>
-      <c r="E408" s="15" t="s">
+      <c r="E408" s="20" t="s">
         <v>777</v>
       </c>
       <c r="F408" s="16"/>
@@ -28392,7 +28392,7 @@
       <c r="D410" s="14" t="s">
         <v>782</v>
       </c>
-      <c r="E410" s="15" t="s">
+      <c r="E410" s="20" t="s">
         <v>783</v>
       </c>
       <c r="F410" s="16"/>
@@ -28434,7 +28434,7 @@
       <c r="D411" s="14" t="s">
         <v>785</v>
       </c>
-      <c r="E411" s="15" t="s">
+      <c r="E411" s="20" t="s">
         <v>786</v>
       </c>
       <c r="F411" s="16"/>
@@ -28476,7 +28476,7 @@
       <c r="D412" s="14" t="s">
         <v>788</v>
       </c>
-      <c r="E412" s="15" t="s">
+      <c r="E412" s="20" t="s">
         <v>789</v>
       </c>
       <c r="F412" s="16"/>
@@ -28518,7 +28518,7 @@
       <c r="D413" s="14" t="s">
         <v>791</v>
       </c>
-      <c r="E413" s="15" t="s">
+      <c r="E413" s="20" t="s">
         <v>792</v>
       </c>
       <c r="F413" s="16"/>
@@ -28636,7 +28636,7 @@
       <c r="D416" s="14" t="s">
         <v>797</v>
       </c>
-      <c r="E416" s="15" t="s">
+      <c r="E416" s="20" t="s">
         <v>798</v>
       </c>
       <c r="F416" s="16"/>
@@ -28678,7 +28678,7 @@
       <c r="D417" s="14" t="s">
         <v>800</v>
       </c>
-      <c r="E417" s="15" t="s">
+      <c r="E417" s="20" t="s">
         <v>801</v>
       </c>
       <c r="F417" s="16"/>
@@ -28930,7 +28930,7 @@
       <c r="D424" s="14" t="s">
         <v>808</v>
       </c>
-      <c r="E424" s="15" t="s">
+      <c r="E424" s="20" t="s">
         <v>809</v>
       </c>
       <c r="F424" s="16"/>
@@ -29040,7 +29040,7 @@
       <c r="D427" s="14" t="s">
         <v>813</v>
       </c>
-      <c r="E427" s="15" t="s">
+      <c r="E427" s="20" t="s">
         <v>814</v>
       </c>
       <c r="F427" s="16"/>
@@ -29082,7 +29082,7 @@
       <c r="D428" s="14" t="s">
         <v>816</v>
       </c>
-      <c r="E428" s="15" t="s">
+      <c r="E428" s="20" t="s">
         <v>817</v>
       </c>
       <c r="F428" s="16"/>
@@ -29200,7 +29200,7 @@
       <c r="D431" s="14" t="s">
         <v>822</v>
       </c>
-      <c r="E431" s="15" t="s">
+      <c r="E431" s="20" t="s">
         <v>823</v>
       </c>
       <c r="F431" s="16"/>
@@ -29242,7 +29242,7 @@
       <c r="D432" s="14" t="s">
         <v>825</v>
       </c>
-      <c r="E432" s="15" t="s">
+      <c r="E432" s="20" t="s">
         <v>826</v>
       </c>
       <c r="F432" s="16"/>
@@ -29284,7 +29284,7 @@
       <c r="D433" s="14" t="s">
         <v>828</v>
       </c>
-      <c r="E433" s="15" t="s">
+      <c r="E433" s="20" t="s">
         <v>829</v>
       </c>
       <c r="F433" s="16"/>
@@ -29326,7 +29326,7 @@
       <c r="D434" s="14" t="s">
         <v>831</v>
       </c>
-      <c r="E434" s="15" t="s">
+      <c r="E434" s="20" t="s">
         <v>832</v>
       </c>
       <c r="F434" s="16"/>
@@ -29368,7 +29368,7 @@
       <c r="D435" s="14" t="s">
         <v>834</v>
       </c>
-      <c r="E435" s="15" t="s">
+      <c r="E435" s="20" t="s">
         <v>835</v>
       </c>
       <c r="F435" s="16"/>
@@ -29562,7 +29562,7 @@
       <c r="D440" s="14" t="s">
         <v>843</v>
       </c>
-      <c r="E440" s="15" t="s">
+      <c r="E440" s="20" t="s">
         <v>844</v>
       </c>
       <c r="F440" s="16"/>
@@ -29638,7 +29638,7 @@
       <c r="D442" s="14" t="s">
         <v>791</v>
       </c>
-      <c r="E442" s="15" t="s">
+      <c r="E442" s="20" t="s">
         <v>847</v>
       </c>
       <c r="F442" s="16"/>
@@ -29720,7 +29720,7 @@
         <v>781</v>
       </c>
       <c r="D444" s="14"/>
-      <c r="E444" s="15" t="s">
+      <c r="E444" s="20" t="s">
         <v>801</v>
       </c>
       <c r="F444" s="16"/>
@@ -29804,7 +29804,7 @@
       <c r="D446" s="14" t="s">
         <v>854</v>
       </c>
-      <c r="E446" s="15" t="s">
+      <c r="E446" s="20" t="s">
         <v>855</v>
       </c>
       <c r="F446" s="16"/>
@@ -29846,7 +29846,7 @@
       <c r="D447" s="14" t="s">
         <v>857</v>
       </c>
-      <c r="E447" s="15" t="s">
+      <c r="E447" s="20" t="s">
         <v>858</v>
       </c>
       <c r="F447" s="16"/>
@@ -29888,7 +29888,7 @@
       <c r="D448" s="14" t="s">
         <v>860</v>
       </c>
-      <c r="E448" s="15" t="s">
+      <c r="E448" s="20" t="s">
         <v>861</v>
       </c>
       <c r="F448" s="16"/>
@@ -29930,7 +29930,7 @@
       <c r="D449" s="14" t="s">
         <v>816</v>
       </c>
-      <c r="E449" s="15" t="s">
+      <c r="E449" s="20" t="s">
         <v>863</v>
       </c>
       <c r="F449" s="16"/>
@@ -29972,7 +29972,7 @@
       <c r="D450" s="14" t="s">
         <v>865</v>
       </c>
-      <c r="E450" s="15" t="s">
+      <c r="E450" s="20" t="s">
         <v>866</v>
       </c>
       <c r="F450" s="16"/>
@@ -30014,7 +30014,7 @@
       <c r="D451" s="14" t="s">
         <v>868</v>
       </c>
-      <c r="E451" s="15" t="s">
+      <c r="E451" s="20" t="s">
         <v>869</v>
       </c>
       <c r="F451" s="16"/>
@@ -30056,7 +30056,7 @@
       <c r="D452" s="14" t="s">
         <v>871</v>
       </c>
-      <c r="E452" s="15" t="s">
+      <c r="E452" s="20" t="s">
         <v>872</v>
       </c>
       <c r="F452" s="16"/>
@@ -30098,7 +30098,7 @@
       <c r="D453" s="14" t="s">
         <v>854</v>
       </c>
-      <c r="E453" s="15" t="s">
+      <c r="E453" s="20" t="s">
         <v>855</v>
       </c>
       <c r="F453" s="16"/>
@@ -30174,7 +30174,7 @@
       <c r="D455" s="14" t="s">
         <v>875</v>
       </c>
-      <c r="E455" s="15" t="s">
+      <c r="E455" s="20" t="s">
         <v>876</v>
       </c>
       <c r="F455" s="16"/>
@@ -30216,7 +30216,7 @@
       <c r="D456" s="14" t="s">
         <v>877</v>
       </c>
-      <c r="E456" s="15" t="s">
+      <c r="E456" s="20" t="s">
         <v>878</v>
       </c>
       <c r="F456" s="16"/>
@@ -30292,7 +30292,7 @@
       <c r="D458" s="14" t="s">
         <v>881</v>
       </c>
-      <c r="E458" s="15" t="s">
+      <c r="E458" s="20" t="s">
         <v>882</v>
       </c>
       <c r="F458" s="16"/>
@@ -30334,7 +30334,7 @@
       <c r="D459" s="14" t="s">
         <v>884</v>
       </c>
-      <c r="E459" s="15" t="s">
+      <c r="E459" s="20" t="s">
         <v>885</v>
       </c>
       <c r="F459" s="16"/>
@@ -30418,7 +30418,7 @@
       <c r="D461" s="14" t="s">
         <v>889</v>
       </c>
-      <c r="E461" s="15" t="s">
+      <c r="E461" s="20" t="s">
         <v>890</v>
       </c>
       <c r="F461" s="16"/>
@@ -30460,7 +30460,7 @@
       <c r="D462" s="14" t="s">
         <v>892</v>
       </c>
-      <c r="E462" s="15" t="s">
+      <c r="E462" s="20" t="s">
         <v>893</v>
       </c>
       <c r="F462" s="16"/>
@@ -30542,7 +30542,7 @@
         <v>781</v>
       </c>
       <c r="D464" s="14"/>
-      <c r="E464" s="15" t="s">
+      <c r="E464" s="20" t="s">
         <v>896</v>
       </c>
       <c r="F464" s="16"/>
@@ -30584,7 +30584,7 @@
       <c r="D465" s="14" t="s">
         <v>898</v>
       </c>
-      <c r="E465" s="15" t="s">
+      <c r="E465" s="20" t="s">
         <v>899</v>
       </c>
       <c r="F465" s="16"/>
@@ -30626,7 +30626,7 @@
       <c r="D466" s="14" t="s">
         <v>892</v>
       </c>
-      <c r="E466" s="15" t="s">
+      <c r="E466" s="20" t="s">
         <v>901</v>
       </c>
       <c r="F466" s="16"/>
@@ -30812,7 +30812,7 @@
       <c r="D471" s="14" t="s">
         <v>908</v>
       </c>
-      <c r="E471" s="15" t="s">
+      <c r="E471" s="20" t="s">
         <v>909</v>
       </c>
       <c r="F471" s="16"/>
@@ -30854,7 +30854,7 @@
       <c r="D472" s="14" t="s">
         <v>911</v>
       </c>
-      <c r="E472" s="15" t="s">
+      <c r="E472" s="20" t="s">
         <v>912</v>
       </c>
       <c r="F472" s="16"/>
@@ -30896,7 +30896,7 @@
       <c r="D473" s="14" t="s">
         <v>875</v>
       </c>
-      <c r="E473" s="15" t="s">
+      <c r="E473" s="20" t="s">
         <v>913</v>
       </c>
       <c r="F473" s="16"/>
@@ -30938,7 +30938,7 @@
       <c r="D474" s="14" t="s">
         <v>915</v>
       </c>
-      <c r="E474" s="15" t="s">
+      <c r="E474" s="20" t="s">
         <v>916</v>
       </c>
       <c r="F474" s="16"/>
@@ -30980,7 +30980,7 @@
       <c r="D475" s="14" t="s">
         <v>889</v>
       </c>
-      <c r="E475" s="15" t="s">
+      <c r="E475" s="20" t="s">
         <v>918</v>
       </c>
       <c r="F475" s="16"/>
@@ -31022,7 +31022,7 @@
       <c r="D476" s="14" t="s">
         <v>920</v>
       </c>
-      <c r="E476" s="15" t="s">
+      <c r="E476" s="20" t="s">
         <v>921</v>
       </c>
       <c r="F476" s="16"/>
@@ -31166,7 +31166,7 @@
       <c r="D480" s="14" t="s">
         <v>923</v>
       </c>
-      <c r="E480" s="15" t="s">
+      <c r="E480" s="20" t="s">
         <v>924</v>
       </c>
       <c r="F480" s="16"/>
@@ -31250,7 +31250,7 @@
       <c r="D482" s="14" t="s">
         <v>928</v>
       </c>
-      <c r="E482" s="15" t="s">
+      <c r="E482" s="20" t="s">
         <v>929</v>
       </c>
       <c r="F482" s="16"/>
@@ -31292,7 +31292,7 @@
       <c r="D483" s="14" t="s">
         <v>931</v>
       </c>
-      <c r="E483" s="15" t="s">
+      <c r="E483" s="20" t="s">
         <v>932</v>
       </c>
       <c r="F483" s="16"/>
@@ -31334,7 +31334,7 @@
       <c r="D484" s="14" t="s">
         <v>934</v>
       </c>
-      <c r="E484" s="15" t="s">
+      <c r="E484" s="20" t="s">
         <v>935</v>
       </c>
       <c r="F484" s="16"/>
@@ -31376,7 +31376,7 @@
       <c r="D485" s="14" t="s">
         <v>828</v>
       </c>
-      <c r="E485" s="15" t="s">
+      <c r="E485" s="20" t="s">
         <v>829</v>
       </c>
       <c r="F485" s="16"/>
@@ -31418,7 +31418,7 @@
       <c r="D486" s="14" t="s">
         <v>938</v>
       </c>
-      <c r="E486" s="15" t="s">
+      <c r="E486" s="20" t="s">
         <v>939</v>
       </c>
       <c r="F486" s="16"/>
@@ -31460,7 +31460,7 @@
       <c r="D487" s="14" t="s">
         <v>941</v>
       </c>
-      <c r="E487" s="15" t="s">
+      <c r="E487" s="20" t="s">
         <v>942</v>
       </c>
       <c r="F487" s="16"/>
@@ -31502,7 +31502,7 @@
       <c r="D488" s="14" t="s">
         <v>915</v>
       </c>
-      <c r="E488" s="15" t="s">
+      <c r="E488" s="20" t="s">
         <v>944</v>
       </c>
       <c r="F488" s="16"/>
@@ -31544,7 +31544,7 @@
       <c r="D489" s="14" t="s">
         <v>946</v>
       </c>
-      <c r="E489" s="15" t="s">
+      <c r="E489" s="20" t="s">
         <v>947</v>
       </c>
       <c r="F489" s="16"/>
@@ -31628,7 +31628,7 @@
       <c r="D491" s="14" t="s">
         <v>950</v>
       </c>
-      <c r="E491" s="15" t="s">
+      <c r="E491" s="20" t="s">
         <v>951</v>
       </c>
       <c r="F491" s="16"/>
@@ -31670,7 +31670,7 @@
       <c r="D492" s="14" t="s">
         <v>953</v>
       </c>
-      <c r="E492" s="15" t="s">
+      <c r="E492" s="20" t="s">
         <v>954</v>
       </c>
       <c r="F492" s="16"/>
@@ -31754,7 +31754,7 @@
       <c r="D494" s="14" t="s">
         <v>941</v>
       </c>
-      <c r="E494" s="15" t="s">
+      <c r="E494" s="20" t="s">
         <v>958</v>
       </c>
       <c r="F494" s="16"/>
@@ -31796,7 +31796,7 @@
       <c r="D495" s="14" t="s">
         <v>960</v>
       </c>
-      <c r="E495" s="15" t="s">
+      <c r="E495" s="20" t="s">
         <v>961</v>
       </c>
       <c r="F495" s="16"/>
@@ -31880,7 +31880,7 @@
       <c r="D497" s="14" t="s">
         <v>964</v>
       </c>
-      <c r="E497" s="15" t="s">
+      <c r="E497" s="20" t="s">
         <v>965</v>
       </c>
       <c r="F497" s="16"/>
@@ -31922,7 +31922,7 @@
       <c r="D498" s="14" t="s">
         <v>967</v>
       </c>
-      <c r="E498" s="15" t="s">
+      <c r="E498" s="20" t="s">
         <v>968</v>
       </c>
       <c r="F498" s="16"/>
@@ -31964,7 +31964,7 @@
       <c r="D499" s="14" t="s">
         <v>970</v>
       </c>
-      <c r="E499" s="15" t="s">
+      <c r="E499" s="20" t="s">
         <v>971</v>
       </c>
       <c r="F499" s="16"/>
@@ -32006,7 +32006,7 @@
       <c r="D500" s="14" t="s">
         <v>972</v>
       </c>
-      <c r="E500" s="15" t="s">
+      <c r="E500" s="20" t="s">
         <v>973</v>
       </c>
       <c r="F500" s="16"/>
@@ -32048,7 +32048,7 @@
       <c r="D501" s="14" t="s">
         <v>975</v>
       </c>
-      <c r="E501" s="15" t="s">
+      <c r="E501" s="20" t="s">
         <v>976</v>
       </c>
       <c r="F501" s="16"/>
@@ -32090,7 +32090,7 @@
       <c r="D502" s="14" t="s">
         <v>843</v>
       </c>
-      <c r="E502" s="15" t="s">
+      <c r="E502" s="20" t="s">
         <v>844</v>
       </c>
       <c r="F502" s="16"/>
@@ -32132,7 +32132,7 @@
       <c r="D503" s="14" t="s">
         <v>938</v>
       </c>
-      <c r="E503" s="15" t="s">
+      <c r="E503" s="20" t="s">
         <v>939</v>
       </c>
       <c r="F503" s="16"/>
@@ -32174,7 +32174,7 @@
       <c r="D504" s="14" t="s">
         <v>980</v>
       </c>
-      <c r="E504" s="15" t="s">
+      <c r="E504" s="20" t="s">
         <v>981</v>
       </c>
       <c r="F504" s="16"/>
@@ -32216,7 +32216,7 @@
       <c r="D505" s="14" t="s">
         <v>915</v>
       </c>
-      <c r="E505" s="15" t="s">
+      <c r="E505" s="20" t="s">
         <v>944</v>
       </c>
       <c r="F505" s="16"/>
@@ -32258,7 +32258,7 @@
       <c r="D506" s="14" t="s">
         <v>820</v>
       </c>
-      <c r="E506" s="15" t="s">
+      <c r="E506" s="20" t="s">
         <v>984</v>
       </c>
       <c r="F506" s="16"/>
@@ -32300,7 +32300,7 @@
       <c r="D507" s="14" t="s">
         <v>791</v>
       </c>
-      <c r="E507" s="15" t="s">
+      <c r="E507" s="20" t="s">
         <v>847</v>
       </c>
       <c r="F507" s="16"/>
@@ -32426,7 +32426,7 @@
       <c r="D510" s="14" t="s">
         <v>990</v>
       </c>
-      <c r="E510" s="15" t="s">
+      <c r="E510" s="20" t="s">
         <v>991</v>
       </c>
       <c r="F510" s="16"/>
@@ -32468,7 +32468,7 @@
       <c r="D511" s="14" t="s">
         <v>993</v>
       </c>
-      <c r="E511" s="15" t="s">
+      <c r="E511" s="20" t="s">
         <v>994</v>
       </c>
       <c r="F511" s="16"/>
@@ -32594,7 +32594,7 @@
       <c r="D514" s="14" t="s">
         <v>1000</v>
       </c>
-      <c r="E514" s="15" t="s">
+      <c r="E514" s="20" t="s">
         <v>1001</v>
       </c>
       <c r="F514" s="16"/>
@@ -32788,7 +32788,7 @@
       <c r="D519" s="14" t="s">
         <v>1008</v>
       </c>
-      <c r="E519" s="15" t="s">
+      <c r="E519" s="20" t="s">
         <v>1009</v>
       </c>
       <c r="F519" s="16"/>
@@ -32830,7 +32830,7 @@
       <c r="D520" s="14" t="s">
         <v>1011</v>
       </c>
-      <c r="E520" s="15" t="s">
+      <c r="E520" s="20" t="s">
         <v>1012</v>
       </c>
       <c r="F520" s="16"/>
@@ -32872,7 +32872,7 @@
       <c r="D521" s="14" t="s">
         <v>788</v>
       </c>
-      <c r="E521" s="15" t="s">
+      <c r="E521" s="20" t="s">
         <v>1014</v>
       </c>
       <c r="F521" s="16"/>
@@ -32914,7 +32914,7 @@
       <c r="D522" s="14" t="s">
         <v>1016</v>
       </c>
-      <c r="E522" s="15" t="s">
+      <c r="E522" s="20" t="s">
         <v>1017</v>
       </c>
       <c r="F522" s="16"/>
@@ -62516,7 +62516,7 @@
       <c r="D1328" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1328" s="15" t="s">
+      <c r="E1328" s="20" t="s">
         <v>2130</v>
       </c>
       <c r="F1328" s="16" t="s">
@@ -62560,7 +62560,7 @@
       <c r="D1329" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1329" s="15" t="s">
+      <c r="E1329" s="20" t="s">
         <v>2134</v>
       </c>
       <c r="F1329" s="16" t="s">
@@ -62604,7 +62604,7 @@
       <c r="D1330" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1330" s="15" t="s">
+      <c r="E1330" s="20" t="s">
         <v>2136</v>
       </c>
       <c r="F1330" s="16" t="s">
@@ -62648,7 +62648,7 @@
       <c r="D1331" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1331" s="15" t="s">
+      <c r="E1331" s="20" t="s">
         <v>2138</v>
       </c>
       <c r="F1331" s="16" t="s">
@@ -62692,7 +62692,7 @@
       <c r="D1332" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1332" s="15" t="s">
+      <c r="E1332" s="20" t="s">
         <v>2140</v>
       </c>
       <c r="F1332" s="16" t="s">
@@ -62736,7 +62736,7 @@
       <c r="D1333" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1333" s="15" t="s">
+      <c r="E1333" s="20" t="s">
         <v>2142</v>
       </c>
       <c r="F1333" s="16" t="s">
@@ -62848,7 +62848,7 @@
       <c r="D1336" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1336" s="15" t="s">
+      <c r="E1336" s="20" t="s">
         <v>2145</v>
       </c>
       <c r="F1336" s="16" t="s">
@@ -62892,7 +62892,7 @@
       <c r="D1337" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1337" s="15" t="s">
+      <c r="E1337" s="20" t="s">
         <v>2147</v>
       </c>
       <c r="F1337" s="16" t="s">
@@ -62936,7 +62936,7 @@
       <c r="D1338" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1338" s="15" t="s">
+      <c r="E1338" s="20" t="s">
         <v>2149</v>
       </c>
       <c r="F1338" s="16" t="s">
@@ -62980,7 +62980,7 @@
       <c r="D1339" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1339" s="15" t="s">
+      <c r="E1339" s="20" t="s">
         <v>2151</v>
       </c>
       <c r="F1339" s="16" t="s">
@@ -63024,7 +63024,7 @@
       <c r="D1340" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1340" s="15" t="s">
+      <c r="E1340" s="20" t="s">
         <v>2153</v>
       </c>
       <c r="F1340" s="16" t="s">
@@ -63068,7 +63068,7 @@
       <c r="D1341" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1341" s="15" t="s">
+      <c r="E1341" s="20" t="s">
         <v>2155</v>
       </c>
       <c r="F1341" s="16" t="s">
@@ -63114,7 +63114,7 @@
       <c r="D1342" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1342" s="15" t="s">
+      <c r="E1342" s="20" t="s">
         <v>2158</v>
       </c>
       <c r="F1342" s="16" t="s">
@@ -63158,7 +63158,7 @@
       <c r="D1343" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1343" s="15" t="s">
+      <c r="E1343" s="20" t="s">
         <v>2160</v>
       </c>
       <c r="F1343" s="16" t="s">
@@ -63202,7 +63202,7 @@
       <c r="D1344" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1344" s="15" t="s">
+      <c r="E1344" s="20" t="s">
         <v>2162</v>
       </c>
       <c r="F1344" s="16" t="s">
@@ -63246,7 +63246,7 @@
       <c r="D1345" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1345" s="15" t="s">
+      <c r="E1345" s="20" t="s">
         <v>2164</v>
       </c>
       <c r="F1345" s="16" t="s">
@@ -63324,7 +63324,7 @@
       <c r="D1347" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1347" s="15" t="s">
+      <c r="E1347" s="20" t="s">
         <v>2166</v>
       </c>
       <c r="F1347" s="16" t="s">
@@ -63368,7 +63368,7 @@
       <c r="D1348" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1348" s="15" t="s">
+      <c r="E1348" s="20" t="s">
         <v>2168</v>
       </c>
       <c r="F1348" s="16" t="s">
@@ -63412,7 +63412,7 @@
       <c r="D1349" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1349" s="15" t="s">
+      <c r="E1349" s="20" t="s">
         <v>2170</v>
       </c>
       <c r="F1349" s="16" t="s">
@@ -63456,7 +63456,7 @@
       <c r="D1350" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1350" s="15" t="s">
+      <c r="E1350" s="20" t="s">
         <v>2172</v>
       </c>
       <c r="F1350" s="16" t="s">
@@ -63502,7 +63502,7 @@
       <c r="D1351" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1351" s="15" t="s">
+      <c r="E1351" s="20" t="s">
         <v>2175</v>
       </c>
       <c r="F1351" s="16" t="s">
@@ -63546,7 +63546,7 @@
       <c r="D1352" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1352" s="15" t="s">
+      <c r="E1352" s="20" t="s">
         <v>2177</v>
       </c>
       <c r="F1352" s="16" t="s">
@@ -63590,7 +63590,7 @@
       <c r="D1353" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1353" s="15" t="s">
+      <c r="E1353" s="20" t="s">
         <v>2180</v>
       </c>
       <c r="F1353" s="16" t="s">
@@ -63678,7 +63678,7 @@
       <c r="D1355" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1355" s="15" t="s">
+      <c r="E1355" s="20" t="s">
         <v>2183</v>
       </c>
       <c r="F1355" s="16" t="s">
@@ -63722,7 +63722,7 @@
       <c r="D1356" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1356" s="15" t="s">
+      <c r="E1356" s="20" t="s">
         <v>2185</v>
       </c>
       <c r="F1356" s="16" t="s">
@@ -63766,7 +63766,7 @@
       <c r="D1357" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1357" s="15" t="s">
+      <c r="E1357" s="20" t="s">
         <v>2187</v>
       </c>
       <c r="F1357" s="16" t="s">
@@ -63810,7 +63810,7 @@
       <c r="D1358" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1358" s="15" t="s">
+      <c r="E1358" s="20" t="s">
         <v>2190</v>
       </c>
       <c r="F1358" s="16" t="s">
@@ -63854,7 +63854,7 @@
       <c r="D1359" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1359" s="15" t="s">
+      <c r="E1359" s="20" t="s">
         <v>2193</v>
       </c>
       <c r="F1359" s="16" t="s">
@@ -63900,7 +63900,7 @@
       <c r="D1360" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1360" s="15" t="s">
+      <c r="E1360" s="20" t="s">
         <v>2196</v>
       </c>
       <c r="F1360" s="16" t="s">
@@ -63944,7 +63944,7 @@
       <c r="D1361" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1361" s="15" t="s">
+      <c r="E1361" s="20" t="s">
         <v>2198</v>
       </c>
       <c r="F1361" s="16" t="s">
@@ -63990,7 +63990,7 @@
       <c r="D1362" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1362" s="15" t="s">
+      <c r="E1362" s="20" t="s">
         <v>2201</v>
       </c>
       <c r="F1362" s="16" t="s">
@@ -64034,7 +64034,7 @@
       <c r="D1363" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1363" s="15" t="s">
+      <c r="E1363" s="20" t="s">
         <v>2203</v>
       </c>
       <c r="F1363" s="16" t="s">
@@ -64078,7 +64078,7 @@
       <c r="D1364" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1364" s="15" t="s">
+      <c r="E1364" s="20" t="s">
         <v>2205</v>
       </c>
       <c r="F1364" s="16" t="s">
@@ -64122,7 +64122,7 @@
       <c r="D1365" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1365" s="15" t="s">
+      <c r="E1365" s="20" t="s">
         <v>2207</v>
       </c>
       <c r="F1365" s="16" t="s">
@@ -64166,7 +64166,7 @@
       <c r="D1366" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1366" s="15" t="s">
+      <c r="E1366" s="20" t="s">
         <v>2209</v>
       </c>
       <c r="F1366" s="16" t="s">
@@ -64210,7 +64210,7 @@
       <c r="D1367" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1367" s="15" t="s">
+      <c r="E1367" s="20" t="s">
         <v>2211</v>
       </c>
       <c r="F1367" s="16" t="s">
@@ -64254,7 +64254,7 @@
       <c r="D1368" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1368" s="15" t="s">
+      <c r="E1368" s="20" t="s">
         <v>2213</v>
       </c>
       <c r="F1368" s="16" t="s">
@@ -64298,7 +64298,7 @@
       <c r="D1369" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1369" s="15" t="s">
+      <c r="E1369" s="20" t="s">
         <v>2215</v>
       </c>
       <c r="F1369" s="16" t="s">
@@ -64342,7 +64342,7 @@
       <c r="D1370" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1370" s="15" t="s">
+      <c r="E1370" s="20" t="s">
         <v>2217</v>
       </c>
       <c r="F1370" s="16" t="s">
@@ -64388,7 +64388,7 @@
       <c r="D1371" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1371" s="15" t="s">
+      <c r="E1371" s="20" t="s">
         <v>2220</v>
       </c>
       <c r="F1371" s="16" t="s">
@@ -64432,7 +64432,7 @@
       <c r="D1372" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E1372" s="15" t="s">
+      <c r="E1372" s="20" t="s">
         <v>2222</v>
       </c>
       <c r="F1372" s="16" t="s">

</xml_diff>